<commit_message>
creation du compte rendu.
</commit_message>
<xml_diff>
--- a/Brief/Modèle-audit-SEO.xlsx
+++ b/Brief/Modèle-audit-SEO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edwin\Documents\GitHub\Projet 4-La Panthere\Brief\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A0210ED-AE68-4E4E-8D01-4B6819693CE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EA6EA41-DF42-4F17-96E9-3D2D113B03AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="94">
   <si>
     <t>Catégorie</t>
   </si>
@@ -310,6 +310,9 @@
   </si>
   <si>
     <t>Correction des ratio img</t>
+  </si>
+  <si>
+    <t>Fichier robot,txt</t>
   </si>
 </sst>
 </file>
@@ -636,7 +639,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="G14" sqref="F14:G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1046,7 +1049,11 @@
         <v>92</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B26" s="6" t="s">
+        <v>93</v>
+      </c>
+    </row>
     <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>